<commit_message>
updated templates with dropdown lists, new field names, sort for type NA fixed
</commit_message>
<xml_diff>
--- a/DIA/QK/Massnahmen.xlsx
+++ b/DIA/QK/Massnahmen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Home$/Repositories/shiny-server/DIA/QK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2408B30-C62E-4F48-A766-7A6666729A53}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54EA197-994C-D545-913C-C9F6C5331A33}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8980" yWindow="12140" windowWidth="40560" windowHeight="12920" tabRatio="692" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,27 +41,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Massnahmen</t>
-  </si>
-  <si>
-    <t>falsch</t>
-  </si>
-  <si>
-    <t>Specimen ID</t>
-  </si>
-  <si>
-    <t>Distribution Nr.</t>
   </si>
   <si>
     <t>Bemerkungen</t>
   </si>
   <si>
-    <t>xxx</t>
+    <t>Bewertung</t>
   </si>
   <si>
-    <t>Bewertung</t>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Specimen</t>
   </si>
 </sst>
 </file>
@@ -550,7 +544,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -563,34 +557,24 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1234</v>
-      </c>
-      <c r="B2" s="4">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>

</xml_diff>